<commit_message>
a few more edits
</commit_message>
<xml_diff>
--- a/logger image/runtimes.xlsx
+++ b/logger image/runtimes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="348" windowWidth="22752" windowHeight="10272" activeTab="2"/>
+    <workbookView xWindow="720" yWindow="348" windowWidth="22752" windowHeight="10272" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,10 +73,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="143"/>
+      <c14:style val="135"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="43"/>
+      <c:style val="35"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -5028,11 +5028,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190695424"/>
-        <c:axId val="161184512"/>
+        <c:axId val="139578368"/>
+        <c:axId val="160482432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190695424"/>
+        <c:axId val="139578368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5042,17 +5042,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="161184512"/>
+        <c:crossAx val="160482432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5062,7 +5052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161184512"/>
+        <c:axId val="160482432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5076,10 +5066,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400"/>
+                  <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:rPr lang="en-US"/>
                   <a:t>AMPS</a:t>
                 </a:r>
               </a:p>
@@ -5092,17 +5082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="190695424"/>
+        <c:crossAx val="139578368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5119,7 +5099,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5130,7 +5110,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8660423" cy="6286500"/>
+    <xdr:ext cx="8659091" cy="6280727"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -5177,6 +5157,9 @@
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
@@ -5185,7 +5168,7 @@
           <a:r>
             <a:rPr lang="en-US" sz="1600" b="1">
               <a:solidFill>
-                <a:schemeClr val="bg1"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
             <a:t>System cycles on at low stage</a:t>
@@ -5218,7 +5201,7 @@
         </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
           <a:solidFill>
-            <a:schemeClr val="bg1"/>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -5263,7 +5246,7 @@
         </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
           <a:solidFill>
-            <a:schemeClr val="bg1"/>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -5308,7 +5291,7 @@
         </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
           <a:solidFill>
-            <a:schemeClr val="bg1"/>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -5353,7 +5336,7 @@
         </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
           <a:solidFill>
-            <a:schemeClr val="bg1"/>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -5396,6 +5379,9 @@
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
       </cdr:spPr>
       <cdr:txBody>
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
@@ -5468,7 +5454,7 @@
           <a:r>
             <a:rPr lang="en-US" sz="1600" b="1">
               <a:solidFill>
-                <a:schemeClr val="bg1"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
             <a:t>System switches</a:t>
@@ -5476,14 +5462,14 @@
           <a:r>
             <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="bg1"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
             <a:t> from low to high stage capacity during longer cycles/hotter conditions</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1600" b="1">
             <a:solidFill>
-              <a:schemeClr val="bg1"/>
+              <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -5514,7 +5500,7 @@
         </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
           <a:solidFill>
-            <a:schemeClr val="bg1"/>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -5559,7 +5545,7 @@
         </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
           <a:solidFill>
-            <a:schemeClr val="bg1"/>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -5604,7 +5590,7 @@
         </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
           <a:solidFill>
-            <a:schemeClr val="bg1"/>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:tailEnd type="arrow"/>
         </a:ln>
@@ -17068,7 +17054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>